<commit_message>
office machine stuff i forgot to commit
</commit_message>
<xml_diff>
--- a/refs/timeline.xlsx
+++ b/refs/timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\dissertation-proposal\refs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AA210AB-D141-4D67-AEE2-DC25C1C4EE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C768EF0-3A50-4C55-BA8B-DD1DD5281F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20640" yWindow="0" windowWidth="20640" windowHeight="16680" xr2:uid="{530BFBB7-CFE3-472B-AF4A-F9CE3862C3AF}"/>
+    <workbookView xWindow="4224" yWindow="4224" windowWidth="34560" windowHeight="13644" xr2:uid="{530BFBB7-CFE3-472B-AF4A-F9CE3862C3AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Objectives</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Formal statistical analysis</t>
+  </si>
+  <si>
+    <t>Graphical causal modeling</t>
   </si>
 </sst>
 </file>
@@ -304,26 +307,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -335,7 +327,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -343,20 +334,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -672,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3E2C4B-8EA8-4E37-B197-2FF06A266315}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,63 +683,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10">
+      <c r="C1" s="18">
         <v>2023</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10">
+      <c r="D1" s="18"/>
+      <c r="E1" s="18">
         <v>2024</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="11">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="6">
         <v>2025</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="17" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="13"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="14">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -753,10 +750,10 @@
       <c r="E4" s="3"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="15"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="14">
+      <c r="A5" s="9">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -767,91 +764,105 @@
       <c r="E5" s="3"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="15"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="15"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="14">
+      <c r="A7" s="9">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="15"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="14">
+      <c r="A8" s="9">
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="15"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="14">
-        <v>3</v>
+      <c r="A9" s="9">
+        <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="16"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="14">
+      <c r="A10" s="9">
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="17"/>
-    </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -861,6 +872,6 @@
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="landscape" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>